<commit_message>
#9 - application 에 Date Rest 추가
게시글, 댓글의 api를 자동으로 restful 하도록 설정
data rest 세팅 하였음
</commit_message>
<xml_diff>
--- a/document/게시판api설계.xlsx
+++ b/document/게시판api설계.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\=== kh정보교육원 ===\수업\github\project-board\document\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7D7E0B-58B1-4DB8-B441-E53A430D631B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-22230" yWindow="8550" windowWidth="18240" windowHeight="11700" xr2:uid="{150BB030-F946-48D3-B981-83732A1A8391}"/>
+    <workbookView xWindow="-23805" yWindow="8550" windowWidth="18240" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
   <si>
     <t>종류</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -149,10 +143,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>어떤 데이터가 전달 될지 설계</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>id, pw, email, (nickname), etc.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -277,23 +267,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>댓글의 id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>필터: 본문</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>/articles/serach/hashtag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>댓글 id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -554,7 +544,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -606,7 +596,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -800,21 +790,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC0CCA9C-DB04-4579-BB58-C4198D692B8C}">
-  <dimension ref="A1:E26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="2" max="2" width="54.25" customWidth="1"/>
     <col min="3" max="3" width="14.375" customWidth="1"/>
@@ -822,7 +812,7 @@
     <col min="5" max="5" width="35.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="20.25">
       <c r="A1" s="13" t="s">
         <v>5</v>
       </c>
@@ -831,7 +821,7 @@
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
     </row>
-    <row r="2" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="17.25" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -848,7 +838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" s="14" t="s">
         <v>22</v>
       </c>
@@ -865,7 +855,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" s="15"/>
       <c r="B4" t="s">
         <v>9</v>
@@ -878,7 +868,7 @@
       </c>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" s="15"/>
       <c r="B5" t="s">
         <v>10</v>
@@ -891,7 +881,7 @@
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" s="15"/>
       <c r="B6" t="s">
         <v>11</v>
@@ -904,7 +894,7 @@
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" s="15"/>
       <c r="B7" t="s">
         <v>12</v>
@@ -917,7 +907,7 @@
       </c>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" s="15"/>
       <c r="B8" t="s">
         <v>13</v>
@@ -930,7 +920,7 @@
       </c>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" s="15"/>
       <c r="B9" t="s">
         <v>19</v>
@@ -943,10 +933,10 @@
       </c>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="17.25" thickBot="1">
       <c r="A10" s="16"/>
       <c r="B10" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>8</v>
@@ -956,93 +946,104 @@
       </c>
       <c r="E10" s="6"/>
     </row>
-    <row r="12" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E12" t="s">
+    <row r="11" spans="1:5" ht="17.25" thickBot="1"/>
+    <row r="12" spans="1:5">
+      <c r="A12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="2" t="s">
+    <row r="13" spans="1:5">
+      <c r="A13" s="15"/>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="15"/>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="4" t="s">
+      <c r="B14" s="11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="15"/>
       <c r="B15" s="11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="E15" s="12"/>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="15"/>
       <c r="B16" s="11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="12"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="15"/>
       <c r="B17" s="11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="15"/>
       <c r="B18" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>38</v>
@@ -1051,25 +1052,23 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5">
       <c r="A19" s="15"/>
-      <c r="B19" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="12" t="s">
+      <c r="B19" s="7" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="15"/>
       <c r="B20" s="7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>8</v>
@@ -1079,23 +1078,25 @@
       </c>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5">
       <c r="A21" s="15"/>
       <c r="B21" s="7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="15"/>
       <c r="B22" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>8</v>
@@ -1103,73 +1104,58 @@
       <c r="D22" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="15"/>
       <c r="B23" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="15"/>
       <c r="B24" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="15"/>
-      <c r="B25" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="7" t="s">
+    <row r="25" spans="1:5" ht="17.25" thickBot="1">
+      <c r="A25" s="16"/>
+      <c r="B25" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="16"/>
-      <c r="B26" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>60</v>
+      <c r="E25" s="10" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A3:A10"/>
-    <mergeCell ref="A13:A26"/>
+    <mergeCell ref="A12:A25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>